<commit_message>
problèmes dans l'écriture des charts détecté
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -74,6 +74,891 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$5:$J$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$5:$O$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$5:$Y$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$5:$AI$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$5:$AS$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$7:$Y$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$7:$AI$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$7:$AS$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$10:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$10:$AI$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$10:$AS$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50030001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50030002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50030001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$9:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$9:$Y$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$9:$AI$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$9:$AS$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50040001"/>
+        <c:axId val="50040002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50040001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50040002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50040002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50040001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$11:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$11:$Y$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$11:$AI$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$11:$AS$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50050001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50050002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50050001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,59 +1246,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:B12"/>
+  <dimension ref="B3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="3" spans="2:2">
+    <row r="3" spans="2:6">
       <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:2">
+    <row r="4" spans="2:6">
       <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>50</v>
+      </c>
+      <c r="E4">
+        <v>70</v>
+      </c>
+      <c r="F4">
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:2">
+    <row r="5" spans="2:6">
       <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="2:2">
+    <row r="6" spans="2:6">
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="2:2">
+    <row r="7" spans="2:6">
       <c r="B7">
         <v>0</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="2:2">
+    <row r="8" spans="2:6">
       <c r="B8">
         <v>0</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="2:2">
+    <row r="9" spans="2:6">
       <c r="B9">
         <v>0</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="2:2">
+    <row r="10" spans="2:6">
       <c r="B10">
         <v>0</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="2:2">
+    <row r="11" spans="2:6">
       <c r="B11">
         <v>0</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="2:2">
+    <row r="12" spans="2:6">
       <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>0</v>
       </c>
     </row>
@@ -431,5 +1436,6 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correction du positionnement des charts
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -840,13 +840,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -870,13 +870,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -900,13 +900,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>33</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -930,15 +930,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">

</xml_diff>

<commit_message>
vérification des derniers correctifs
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -674,7 +674,7 @@
           <c:order val="0"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$A$11:$E$11</c:f>
+              <c:f>data!$A$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -699,7 +699,7 @@
           <c:order val="1"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$F$11:$J$11</c:f>
+              <c:f>data!$F$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -715,7 +715,7 @@
           <c:order val="2"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$K$11:$O$11</c:f>
+              <c:f>data!$K$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -728,7 +728,7 @@
           <c:order val="3"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$P$11:$Y$11</c:f>
+              <c:f>data!$P$8:$Y$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -741,7 +741,7 @@
           <c:order val="4"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$Z$11:$AI$11</c:f>
+              <c:f>data!$Z$8:$AI$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -754,7 +754,7 @@
           <c:order val="5"/>
           <c:val>
             <c:numRef>
-              <c:f>data!$AJ$11:$AS$11</c:f>
+              <c:f>data!$AJ$8:$AS$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -788,6 +788,298 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50050001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$11:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$11:$Y$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$11:$AI$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$11:$AS$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50060001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50060002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50060001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$6:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$6:$Y$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$6:$AI$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AJ$6:$AS$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50070001"/>
+        <c:axId val="50070002"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="50070001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50070002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50070001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -930,13 +1222,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
@@ -953,6 +1245,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>

</xml_diff>

<commit_message>
fin du 24/06/15 -- total bullshit.
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -12,26 +12,6 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>history10</t>
-  </si>
-  <si>
-    <t>history30</t>
-  </si>
-  <si>
-    <t>history50</t>
-  </si>
-  <si>
-    <t>history70</t>
-  </si>
-  <si>
-    <t>history90</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -114,19 +94,7 @@
               <c:f>data!$A$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>70</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -142,19 +110,7 @@
               <c:f>data!$A$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -170,19 +126,7 @@
               <c:f>data!$A$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -198,19 +142,7 @@
               <c:f>data!$A$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -226,19 +158,7 @@
               <c:f>data!$A$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -254,19 +174,7 @@
               <c:f>data!$A$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -282,19 +190,7 @@
               <c:f>data!$A$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -381,10 +277,7 @@
               <c:f>data!$F$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>90</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -400,10 +293,7 @@
               <c:f>data!$F$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -419,10 +309,7 @@
               <c:f>data!$F$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -438,10 +325,7 @@
               <c:f>data!$F$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -457,10 +341,7 @@
               <c:f>data!$F$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -476,10 +357,7 @@
               <c:f>data!$F$10:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -495,10 +373,7 @@
               <c:f>data!$F$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -585,7 +460,7 @@
               <c:f>data!$AJ$5:$AS$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -601,7 +476,7 @@
               <c:f>data!$AJ$6:$AS$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -617,7 +492,7 @@
               <c:f>data!$AJ$7:$AS$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -633,7 +508,7 @@
               <c:f>data!$AJ$8:$AS$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -649,7 +524,7 @@
               <c:f>data!$AJ$9:$AS$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -665,7 +540,7 @@
               <c:f>data!$AJ$10:$AS$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -681,7 +556,7 @@
               <c:f>data!$AJ$11:$AS$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -768,7 +643,7 @@
               <c:f>data!$Z$5:$AI$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -784,7 +659,7 @@
               <c:f>data!$Z$6:$AI$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -800,7 +675,7 @@
               <c:f>data!$Z$7:$AI$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -816,7 +691,7 @@
               <c:f>data!$Z$8:$AI$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -832,7 +707,7 @@
               <c:f>data!$Z$9:$AI$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -848,7 +723,7 @@
               <c:f>data!$Z$10:$AI$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -864,7 +739,7 @@
               <c:f>data!$Z$11:$AI$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -951,7 +826,7 @@
               <c:f>data!$P$5:$Y$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -967,7 +842,7 @@
               <c:f>data!$P$6:$Y$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -983,7 +858,7 @@
               <c:f>data!$P$7:$Y$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -999,7 +874,7 @@
               <c:f>data!$P$8:$Y$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1015,7 +890,7 @@
               <c:f>data!$P$9:$Y$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1031,7 +906,7 @@
               <c:f>data!$P$10:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1047,7 +922,7 @@
               <c:f>data!$P$11:$Y$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1134,7 +1009,7 @@
               <c:f>data!$K$5:$O$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1150,7 +1025,7 @@
               <c:f>data!$K$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1166,7 +1041,7 @@
               <c:f>data!$K$7:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1182,7 +1057,7 @@
               <c:f>data!$K$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1198,7 +1073,7 @@
               <c:f>data!$K$9:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1214,7 +1089,7 @@
               <c:f>data!$K$10:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1230,7 +1105,7 @@
               <c:f>data!$K$11:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="1"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1373,15 +1248,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1749,183 +1624,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B3:F12"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6">
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>50</v>
-      </c>
-      <c r="E4">
-        <v>70</v>
-      </c>
-      <c r="F4">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>70</v>
-      </c>
-      <c r="F5">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
version fonctionnelle sur ubuntu
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -12,6 +12,26 @@
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>history10</t>
+  </si>
+  <si>
+    <t>history30</t>
+  </si>
+  <si>
+    <t>history50</t>
+  </si>
+  <si>
+    <t>history70</t>
+  </si>
+  <si>
+    <t>history90</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -94,7 +114,19 @@
               <c:f>data!$A$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -110,7 +142,19 @@
               <c:f>data!$A$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -126,7 +170,19 @@
               <c:f>data!$A$7:$E$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -142,7 +198,19 @@
               <c:f>data!$A$8:$E$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -158,7 +226,19 @@
               <c:f>data!$A$9:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -174,7 +254,19 @@
               <c:f>data!$A$10:$E$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -190,7 +282,19 @@
               <c:f>data!$A$11:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="1">
+                  <c:v>-499</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-499</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-499</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -277,7 +381,10 @@
               <c:f>data!$F$5:$J$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>90</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -293,7 +400,10 @@
               <c:f>data!$F$6:$J$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -309,7 +419,10 @@
               <c:f>data!$F$7:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -325,7 +438,10 @@
               <c:f>data!$F$8:$J$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -341,7 +457,10 @@
               <c:f>data!$F$9:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -357,7 +476,10 @@
               <c:f>data!$F$10:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -373,7 +495,10 @@
               <c:f>data!$F$11:$J$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-499</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -460,7 +585,7 @@
               <c:f>data!$AJ$5:$AS$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -476,7 +601,7 @@
               <c:f>data!$AJ$6:$AS$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -492,7 +617,7 @@
               <c:f>data!$AJ$7:$AS$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -508,7 +633,7 @@
               <c:f>data!$AJ$8:$AS$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -524,7 +649,7 @@
               <c:f>data!$AJ$9:$AS$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -540,7 +665,7 @@
               <c:f>data!$AJ$10:$AS$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -556,7 +681,7 @@
               <c:f>data!$AJ$11:$AS$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -643,7 +768,7 @@
               <c:f>data!$Z$5:$AI$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -659,7 +784,7 @@
               <c:f>data!$Z$6:$AI$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -675,7 +800,7 @@
               <c:f>data!$Z$7:$AI$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -691,7 +816,7 @@
               <c:f>data!$Z$8:$AI$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -707,7 +832,7 @@
               <c:f>data!$Z$9:$AI$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -723,7 +848,7 @@
               <c:f>data!$Z$10:$AI$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -739,7 +864,7 @@
               <c:f>data!$Z$11:$AI$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -826,7 +951,7 @@
               <c:f>data!$P$5:$Y$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -842,7 +967,7 @@
               <c:f>data!$P$6:$Y$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -858,7 +983,7 @@
               <c:f>data!$P$7:$Y$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -874,7 +999,7 @@
               <c:f>data!$P$8:$Y$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -890,7 +1015,7 @@
               <c:f>data!$P$9:$Y$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -906,7 +1031,7 @@
               <c:f>data!$P$10:$Y$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -922,7 +1047,7 @@
               <c:f>data!$P$11:$Y$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="10"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1009,7 +1134,7 @@
               <c:f>data!$K$5:$O$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1025,7 +1150,7 @@
               <c:f>data!$K$6:$O$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1041,7 +1166,7 @@
               <c:f>data!$K$7:$O$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1057,7 +1182,7 @@
               <c:f>data!$K$8:$O$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1073,7 +1198,7 @@
               <c:f>data!$K$9:$O$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1089,7 +1214,7 @@
               <c:f>data!$K$10:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1105,7 +1230,7 @@
               <c:f>data!$K$11:$O$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="5"/>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1624,12 +1749,166 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B3:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="2:6">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <v>50</v>
+      </c>
+      <c r="E5">
+        <v>70</v>
+      </c>
+      <c r="F5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6">
+      <c r="B8">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="C8">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="D8">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="E8">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="F8">
+        <v>0.0509259259259259</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6">
+      <c r="B9">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>9</v>
+      </c>
+      <c r="F9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6">
+      <c r="B10">
+        <v>43.2</v>
+      </c>
+      <c r="C10">
+        <v>43.2</v>
+      </c>
+      <c r="D10">
+        <v>43.2</v>
+      </c>
+      <c r="E10">
+        <v>43.2</v>
+      </c>
+      <c r="F10">
+        <v>43.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6">
+      <c r="B11">
+        <v>-499</v>
+      </c>
+      <c r="C11">
+        <v>-499</v>
+      </c>
+      <c r="D11">
+        <v>-499</v>
+      </c>
+      <c r="E11">
+        <v>-499</v>
+      </c>
+      <c r="F11">
+        <v>-499</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6">
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
resultats du second test
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -15,10 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>test</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>history10</t>
   </si>
@@ -118,17 +115,20 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -146,6 +146,71 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>9</c:v>
                 </c:pt>
@@ -163,17 +228,82 @@
           </c:val>
         </c:ser>
         <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:v>fiabilité height</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$7:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-1233</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-1233</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-1233</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1233</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-1233</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -185,118 +315,6 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>proportion de cibles</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$8:$E$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>nombre de points</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$9:$E$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>nombre de pertes</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$10:$E$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>indice de performance</c:v>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$11:$E$11</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="1">
-                  <c:v>-383</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-383</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-383</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -385,9 +403,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>90</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -404,9 +419,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -423,9 +435,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -442,9 +451,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -461,9 +467,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -480,9 +483,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -499,9 +499,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>-383</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1752,167 +1749,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F12"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
       <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>70</v>
+      </c>
+      <c r="E4">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6">
         <v>0</v>
       </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="2:6">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" t="s">
-        <v>5</v>
+    <row r="7" spans="1:5">
+      <c r="A7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="B7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="C7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="D7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="E7">
+        <v>0.0509259259259259</v>
       </c>
     </row>
-    <row r="5" spans="2:6">
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5">
-        <v>30</v>
-      </c>
-      <c r="D5">
-        <v>50</v>
-      </c>
-      <c r="E5">
-        <v>70</v>
-      </c>
-      <c r="F5">
-        <v>90</v>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
-      <c r="B6">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>9</v>
-      </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>9</v>
-      </c>
-      <c r="F6">
-        <v>9</v>
+    <row r="9" spans="1:5">
+      <c r="A9">
+        <v>43.2</v>
+      </c>
+      <c r="B9">
+        <v>43.2</v>
+      </c>
+      <c r="C9">
+        <v>43.2</v>
+      </c>
+      <c r="D9">
+        <v>43.2</v>
+      </c>
+      <c r="E9">
+        <v>43.2</v>
       </c>
     </row>
-    <row r="7" spans="2:6">
-      <c r="B7">
+    <row r="10" spans="1:5">
+      <c r="A10">
+        <v>-1233</v>
+      </c>
+      <c r="B10">
+        <v>-1233</v>
+      </c>
+      <c r="C10">
+        <v>-1233</v>
+      </c>
+      <c r="D10">
+        <v>-1233</v>
+      </c>
+      <c r="E10">
+        <v>-1233</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="B11">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="C11">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="D11">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="C8">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="D8">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="E8">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="F8">
-        <v>0.0509259259259259</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
-      <c r="B9">
-        <v>9</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>9</v>
-      </c>
-      <c r="E9">
-        <v>9</v>
-      </c>
-      <c r="F9">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
-      <c r="B10">
-        <v>43.2</v>
-      </c>
-      <c r="C10">
-        <v>43.2</v>
-      </c>
-      <c r="D10">
-        <v>43.2</v>
-      </c>
-      <c r="E10">
-        <v>43.2</v>
-      </c>
-      <c r="F10">
-        <v>43.2</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6">
-      <c r="B11">
-        <v>-383</v>
-      </c>
-      <c r="C11">
-        <v>-383</v>
-      </c>
-      <c r="D11">
-        <v>-383</v>
-      </c>
       <c r="E11">
-        <v>-383</v>
-      </c>
-      <c r="F11">
-        <v>-383</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fonctionnement de l'ajout des frames
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -271,19 +271,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>-1233</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1233</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-1233</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-1233</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-1233</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,19 +1876,19 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>-1233</v>
+        <v>0</v>
       </c>
       <c r="B10">
-        <v>-1233</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>-1233</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>-1233</v>
+        <v>0</v>
       </c>
       <c r="E10">
-        <v>-1233</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">

</xml_diff>

<commit_message>
generalisation a tous les parametres de la v1
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>history10</t>
   </si>
@@ -30,6 +30,117 @@
   </si>
   <si>
     <t>history90</t>
+  </si>
+  <si>
+    <t>points_min3</t>
+  </si>
+  <si>
+    <t>points_min6</t>
+  </si>
+  <si>
+    <t>points_min9</t>
+  </si>
+  <si>
+    <t>points_min12</t>
+  </si>
+  <si>
+    <t>surface_min5</t>
+  </si>
+  <si>
+    <t>surface_min15</t>
+  </si>
+  <si>
+    <t>surface_min25</t>
+  </si>
+  <si>
+    <t>surface_min35</t>
+  </si>
+  <si>
+    <t>surface_min45</t>
+  </si>
+  <si>
+    <t>between_target100</t>
+  </si>
+  <si>
+    <t>between_target200</t>
+  </si>
+  <si>
+    <t>between_target300</t>
+  </si>
+  <si>
+    <t>between_target400</t>
+  </si>
+  <si>
+    <t>between_target500</t>
+  </si>
+  <si>
+    <t>between_target600</t>
+  </si>
+  <si>
+    <t>between_target700</t>
+  </si>
+  <si>
+    <t>between_target800</t>
+  </si>
+  <si>
+    <t>between_target900</t>
+  </si>
+  <si>
+    <t>distance_3d0.5</t>
+  </si>
+  <si>
+    <t>distance_3d1.0</t>
+  </si>
+  <si>
+    <t>distance_3d1.5</t>
+  </si>
+  <si>
+    <t>distance_3d2.0</t>
+  </si>
+  <si>
+    <t>distance_3d2.5</t>
+  </si>
+  <si>
+    <t>distance_3d3.0</t>
+  </si>
+  <si>
+    <t>distance_3d3.5</t>
+  </si>
+  <si>
+    <t>distance_3d4.0</t>
+  </si>
+  <si>
+    <t>distance_3d4.5</t>
+  </si>
+  <si>
+    <t>size_min2</t>
+  </si>
+  <si>
+    <t>size_min7</t>
+  </si>
+  <si>
+    <t>size_min12</t>
+  </si>
+  <si>
+    <t>size_min17</t>
+  </si>
+  <si>
+    <t>size_min22</t>
+  </si>
+  <si>
+    <t>size_min27</t>
+  </si>
+  <si>
+    <t>size_min32</t>
+  </si>
+  <si>
+    <t>size_min37</t>
+  </si>
+  <si>
+    <t>size_min42</t>
+  </si>
+  <si>
+    <t>size_min47</t>
   </si>
 </sst>
 </file>
@@ -271,19 +382,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -403,6 +514,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -419,6 +545,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -435,6 +576,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -451,6 +607,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -467,6 +638,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -483,6 +669,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -499,6 +700,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -586,6 +802,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -602,6 +839,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -618,6 +876,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -634,6 +913,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -650,6 +950,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -666,6 +987,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>509</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -682,6 +1024,27 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -769,6 +1132,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -785,6 +1178,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -801,6 +1224,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -817,6 +1270,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -833,6 +1316,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -849,6 +1362,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>509</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -865,6 +1408,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -952,6 +1525,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -968,6 +1571,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -984,6 +1617,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1000,6 +1663,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1016,6 +1709,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1032,6 +1755,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>509</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1048,6 +1801,36 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1135,6 +1918,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1151,6 +1949,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1167,6 +1980,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0509259259259259</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1183,6 +2011,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1199,6 +2042,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1215,6 +2073,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1231,6 +2104,21 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1749,13 +2637,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:AP11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:42">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1771,8 +2659,119 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2" t="s">
+        <v>20</v>
+      </c>
+      <c r="V2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:42">
       <c r="A4">
         <v>10</v>
       </c>
@@ -1788,8 +2787,119 @@
       <c r="E4">
         <v>90</v>
       </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
+      </c>
+      <c r="H4">
+        <v>9</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>15</v>
+      </c>
+      <c r="L4">
+        <v>25</v>
+      </c>
+      <c r="M4">
+        <v>35</v>
+      </c>
+      <c r="N4">
+        <v>45</v>
+      </c>
+      <c r="O4">
+        <v>100</v>
+      </c>
+      <c r="P4">
+        <v>200</v>
+      </c>
+      <c r="Q4">
+        <v>300</v>
+      </c>
+      <c r="R4">
+        <v>400</v>
+      </c>
+      <c r="S4">
+        <v>500</v>
+      </c>
+      <c r="T4">
+        <v>600</v>
+      </c>
+      <c r="U4">
+        <v>700</v>
+      </c>
+      <c r="V4">
+        <v>800</v>
+      </c>
+      <c r="W4">
+        <v>900</v>
+      </c>
+      <c r="X4">
+        <v>0.5</v>
+      </c>
+      <c r="Y4">
+        <v>1</v>
+      </c>
+      <c r="Z4">
+        <v>1.5</v>
+      </c>
+      <c r="AA4">
+        <v>2</v>
+      </c>
+      <c r="AB4">
+        <v>2.5</v>
+      </c>
+      <c r="AC4">
+        <v>3</v>
+      </c>
+      <c r="AD4">
+        <v>3.5</v>
+      </c>
+      <c r="AE4">
+        <v>4</v>
+      </c>
+      <c r="AF4">
+        <v>4.5</v>
+      </c>
+      <c r="AG4">
+        <v>2</v>
+      </c>
+      <c r="AH4">
+        <v>7</v>
+      </c>
+      <c r="AI4">
+        <v>12</v>
+      </c>
+      <c r="AJ4">
+        <v>17</v>
+      </c>
+      <c r="AK4">
+        <v>22</v>
+      </c>
+      <c r="AL4">
+        <v>27</v>
+      </c>
+      <c r="AM4">
+        <v>32</v>
+      </c>
+      <c r="AN4">
+        <v>37</v>
+      </c>
+      <c r="AO4">
+        <v>42</v>
+      </c>
+      <c r="AP4">
+        <v>47</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:42">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1805,8 +2915,119 @@
       <c r="E5">
         <v>9</v>
       </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>9</v>
+      </c>
+      <c r="H5">
+        <v>9</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>9</v>
+      </c>
+      <c r="K5">
+        <v>9</v>
+      </c>
+      <c r="L5">
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>9</v>
+      </c>
+      <c r="O5">
+        <v>9</v>
+      </c>
+      <c r="P5">
+        <v>9</v>
+      </c>
+      <c r="Q5">
+        <v>9</v>
+      </c>
+      <c r="R5">
+        <v>9</v>
+      </c>
+      <c r="S5">
+        <v>9</v>
+      </c>
+      <c r="T5">
+        <v>9</v>
+      </c>
+      <c r="U5">
+        <v>9</v>
+      </c>
+      <c r="V5">
+        <v>9</v>
+      </c>
+      <c r="W5">
+        <v>9</v>
+      </c>
+      <c r="X5">
+        <v>9</v>
+      </c>
+      <c r="Y5">
+        <v>9</v>
+      </c>
+      <c r="Z5">
+        <v>9</v>
+      </c>
+      <c r="AA5">
+        <v>9</v>
+      </c>
+      <c r="AB5">
+        <v>9</v>
+      </c>
+      <c r="AC5">
+        <v>9</v>
+      </c>
+      <c r="AD5">
+        <v>9</v>
+      </c>
+      <c r="AE5">
+        <v>9</v>
+      </c>
+      <c r="AF5">
+        <v>9</v>
+      </c>
+      <c r="AG5">
+        <v>9</v>
+      </c>
+      <c r="AH5">
+        <v>9</v>
+      </c>
+      <c r="AI5">
+        <v>9</v>
+      </c>
+      <c r="AJ5">
+        <v>9</v>
+      </c>
+      <c r="AK5">
+        <v>9</v>
+      </c>
+      <c r="AL5">
+        <v>9</v>
+      </c>
+      <c r="AM5">
+        <v>9</v>
+      </c>
+      <c r="AN5">
+        <v>9</v>
+      </c>
+      <c r="AO5">
+        <v>9</v>
+      </c>
+      <c r="AP5">
+        <v>9</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:42">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1822,8 +3043,119 @@
       <c r="E6">
         <v>0</v>
       </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6">
+        <v>0</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
+        <v>0</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0</v>
+      </c>
+      <c r="AI6">
+        <v>0</v>
+      </c>
+      <c r="AJ6">
+        <v>0</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:42">
       <c r="A7">
         <v>0.0509259259259259</v>
       </c>
@@ -1839,8 +3171,119 @@
       <c r="E7">
         <v>0.0509259259259259</v>
       </c>
+      <c r="F7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="G7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="H7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="I7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="J7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="K7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="L7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="M7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="N7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="O7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="P7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="Q7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="R7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="S7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="T7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="U7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="V7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="W7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="X7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="Y7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="Z7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AA7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AB7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AC7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AD7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AE7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AF7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AG7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AH7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AI7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AJ7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AK7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AL7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AM7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AN7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AO7">
+        <v>0.0509259259259259</v>
+      </c>
+      <c r="AP7">
+        <v>0.0509259259259259</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:42">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1856,8 +3299,119 @@
       <c r="E8">
         <v>9</v>
       </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>9</v>
+      </c>
+      <c r="H8">
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <v>9</v>
+      </c>
+      <c r="J8">
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <v>9</v>
+      </c>
+      <c r="L8">
+        <v>9</v>
+      </c>
+      <c r="M8">
+        <v>9</v>
+      </c>
+      <c r="N8">
+        <v>9</v>
+      </c>
+      <c r="O8">
+        <v>9</v>
+      </c>
+      <c r="P8">
+        <v>9</v>
+      </c>
+      <c r="Q8">
+        <v>9</v>
+      </c>
+      <c r="R8">
+        <v>9</v>
+      </c>
+      <c r="S8">
+        <v>9</v>
+      </c>
+      <c r="T8">
+        <v>9</v>
+      </c>
+      <c r="U8">
+        <v>9</v>
+      </c>
+      <c r="V8">
+        <v>9</v>
+      </c>
+      <c r="W8">
+        <v>9</v>
+      </c>
+      <c r="X8">
+        <v>9</v>
+      </c>
+      <c r="Y8">
+        <v>9</v>
+      </c>
+      <c r="Z8">
+        <v>9</v>
+      </c>
+      <c r="AA8">
+        <v>9</v>
+      </c>
+      <c r="AB8">
+        <v>9</v>
+      </c>
+      <c r="AC8">
+        <v>9</v>
+      </c>
+      <c r="AD8">
+        <v>9</v>
+      </c>
+      <c r="AE8">
+        <v>9</v>
+      </c>
+      <c r="AF8">
+        <v>9</v>
+      </c>
+      <c r="AG8">
+        <v>9</v>
+      </c>
+      <c r="AH8">
+        <v>9</v>
+      </c>
+      <c r="AI8">
+        <v>9</v>
+      </c>
+      <c r="AJ8">
+        <v>9</v>
+      </c>
+      <c r="AK8">
+        <v>9</v>
+      </c>
+      <c r="AL8">
+        <v>9</v>
+      </c>
+      <c r="AM8">
+        <v>9</v>
+      </c>
+      <c r="AN8">
+        <v>9</v>
+      </c>
+      <c r="AO8">
+        <v>9</v>
+      </c>
+      <c r="AP8">
+        <v>9</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:42">
       <c r="A9">
         <v>43.2</v>
       </c>
@@ -1873,25 +3427,247 @@
       <c r="E9">
         <v>43.2</v>
       </c>
+      <c r="F9">
+        <v>43.2</v>
+      </c>
+      <c r="G9">
+        <v>43.2</v>
+      </c>
+      <c r="H9">
+        <v>43.2</v>
+      </c>
+      <c r="I9">
+        <v>43.2</v>
+      </c>
+      <c r="J9">
+        <v>43.2</v>
+      </c>
+      <c r="K9">
+        <v>43.2</v>
+      </c>
+      <c r="L9">
+        <v>43.2</v>
+      </c>
+      <c r="M9">
+        <v>43.2</v>
+      </c>
+      <c r="N9">
+        <v>43.2</v>
+      </c>
+      <c r="O9">
+        <v>43.2</v>
+      </c>
+      <c r="P9">
+        <v>43.2</v>
+      </c>
+      <c r="Q9">
+        <v>43.2</v>
+      </c>
+      <c r="R9">
+        <v>43.2</v>
+      </c>
+      <c r="S9">
+        <v>43.2</v>
+      </c>
+      <c r="T9">
+        <v>43.2</v>
+      </c>
+      <c r="U9">
+        <v>43.2</v>
+      </c>
+      <c r="V9">
+        <v>43.2</v>
+      </c>
+      <c r="W9">
+        <v>43.2</v>
+      </c>
+      <c r="X9">
+        <v>43.2</v>
+      </c>
+      <c r="Y9">
+        <v>43.2</v>
+      </c>
+      <c r="Z9">
+        <v>43.2</v>
+      </c>
+      <c r="AA9">
+        <v>43.2</v>
+      </c>
+      <c r="AB9">
+        <v>43.2</v>
+      </c>
+      <c r="AC9">
+        <v>43.2</v>
+      </c>
+      <c r="AD9">
+        <v>43.2</v>
+      </c>
+      <c r="AE9">
+        <v>43.2</v>
+      </c>
+      <c r="AF9">
+        <v>43.2</v>
+      </c>
+      <c r="AG9">
+        <v>43.2</v>
+      </c>
+      <c r="AH9">
+        <v>43.2</v>
+      </c>
+      <c r="AI9">
+        <v>43.2</v>
+      </c>
+      <c r="AJ9">
+        <v>43.2</v>
+      </c>
+      <c r="AK9">
+        <v>43.2</v>
+      </c>
+      <c r="AL9">
+        <v>43.2</v>
+      </c>
+      <c r="AM9">
+        <v>43.2</v>
+      </c>
+      <c r="AN9">
+        <v>43.2</v>
+      </c>
+      <c r="AO9">
+        <v>43.2</v>
+      </c>
+      <c r="AP9">
+        <v>43.2</v>
+      </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:42">
       <c r="A10">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>509</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>509</v>
+      </c>
+      <c r="F10">
+        <v>509</v>
+      </c>
+      <c r="G10">
+        <v>509</v>
+      </c>
+      <c r="H10">
+        <v>509</v>
+      </c>
+      <c r="I10">
+        <v>509</v>
+      </c>
+      <c r="J10">
+        <v>509</v>
+      </c>
+      <c r="K10">
+        <v>509</v>
+      </c>
+      <c r="L10">
+        <v>509</v>
+      </c>
+      <c r="M10">
+        <v>509</v>
+      </c>
+      <c r="N10">
+        <v>509</v>
+      </c>
+      <c r="O10">
+        <v>509</v>
+      </c>
+      <c r="P10">
+        <v>509</v>
+      </c>
+      <c r="Q10">
+        <v>509</v>
+      </c>
+      <c r="R10">
+        <v>509</v>
+      </c>
+      <c r="S10">
+        <v>509</v>
+      </c>
+      <c r="T10">
+        <v>509</v>
+      </c>
+      <c r="U10">
+        <v>509</v>
+      </c>
+      <c r="V10">
+        <v>509</v>
+      </c>
+      <c r="W10">
+        <v>509</v>
+      </c>
+      <c r="X10">
+        <v>509</v>
+      </c>
+      <c r="Y10">
+        <v>509</v>
+      </c>
+      <c r="Z10">
+        <v>509</v>
+      </c>
+      <c r="AA10">
+        <v>509</v>
+      </c>
+      <c r="AB10">
+        <v>509</v>
+      </c>
+      <c r="AC10">
+        <v>509</v>
+      </c>
+      <c r="AD10">
+        <v>509</v>
+      </c>
+      <c r="AE10">
+        <v>509</v>
+      </c>
+      <c r="AF10">
+        <v>509</v>
+      </c>
+      <c r="AG10">
+        <v>509</v>
+      </c>
+      <c r="AH10">
+        <v>509</v>
+      </c>
+      <c r="AI10">
+        <v>509</v>
+      </c>
+      <c r="AJ10">
+        <v>509</v>
+      </c>
+      <c r="AK10">
+        <v>509</v>
+      </c>
+      <c r="AL10">
+        <v>509</v>
+      </c>
+      <c r="AM10">
+        <v>509</v>
+      </c>
+      <c r="AN10">
+        <v>509</v>
+      </c>
+      <c r="AO10">
+        <v>509</v>
+      </c>
+      <c r="AP10">
+        <v>509</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:42">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1905,6 +3681,117 @@
         <v>0</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+      <c r="AJ11">
+        <v>0</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <v>0</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adaptation aux parametres de la v2
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -15,141 +15,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
-    <t>history10.0</t>
+    <t>coef15.0</t>
   </si>
   <si>
-    <t>history30.0</t>
+    <t>coef17.0</t>
   </si>
   <si>
-    <t>history50.0</t>
+    <t>coef19.0</t>
   </si>
   <si>
-    <t>history70.0</t>
+    <t>coef111.0</t>
   </si>
   <si>
-    <t>history90.0</t>
+    <t>coef113.0</t>
   </si>
   <si>
-    <t>points_min3.0</t>
+    <t>coef25.0</t>
   </si>
   <si>
-    <t>points_min6.0</t>
+    <t>coef27.0</t>
   </si>
   <si>
-    <t>points_min9.0</t>
+    <t>coef29.0</t>
   </si>
   <si>
-    <t>points_min12.0</t>
+    <t>coef211.0</t>
   </si>
   <si>
-    <t>points_min15.0</t>
+    <t>coef213.0</t>
   </si>
   <si>
-    <t>surface_min5.0</t>
+    <t>coef35.0</t>
   </si>
   <si>
-    <t>surface_min15.0</t>
+    <t>coef37.0</t>
   </si>
   <si>
-    <t>surface_min25.0</t>
+    <t>coef39.0</t>
   </si>
   <si>
-    <t>surface_min35.0</t>
+    <t>coef311.0</t>
   </si>
   <si>
-    <t>surface_min45.0</t>
+    <t>coef313.0</t>
   </si>
   <si>
-    <t>between_target100.0</t>
+    <t>coef45.0</t>
   </si>
   <si>
-    <t>between_target1100.0</t>
+    <t>coef47.0</t>
   </si>
   <si>
-    <t>between_target2100.0</t>
+    <t>coef49.0</t>
   </si>
   <si>
-    <t>between_target3100.0</t>
+    <t>coef411.0</t>
   </si>
   <si>
-    <t>between_target4100.0</t>
+    <t>coef413.0</t>
   </si>
   <si>
-    <t>between_target5100.0</t>
+    <t>coef55.0</t>
   </si>
   <si>
-    <t>between_target6100.0</t>
+    <t>coef57.0</t>
   </si>
   <si>
-    <t>between_target7100.0</t>
+    <t>coef59.0</t>
   </si>
   <si>
-    <t>between_target8100.0</t>
+    <t>coef511.0</t>
   </si>
   <si>
-    <t>between_target9100.0</t>
+    <t>coef513.0</t>
   </si>
   <si>
-    <t>distance_3d0.5</t>
+    <t>coef80.0</t>
   </si>
   <si>
-    <t>distance_3d1.0</t>
+    <t>coef81.0</t>
   </si>
   <si>
-    <t>distance_3d1.5</t>
+    <t>coef82.0</t>
   </si>
   <si>
-    <t>distance_3d2.0</t>
+    <t>coef83.0</t>
   </si>
   <si>
-    <t>distance_3d2.5</t>
+    <t>coef84.0</t>
   </si>
   <si>
-    <t>distance_3d3.0</t>
+    <t>coef125.0</t>
   </si>
   <si>
-    <t>distance_3d3.5</t>
+    <t>coef127.0</t>
   </si>
   <si>
-    <t>distance_3d4.0</t>
+    <t>coef129.0</t>
   </si>
   <si>
-    <t>distance_3d4.5</t>
+    <t>coef1211.0</t>
   </si>
   <si>
-    <t>distance_3d5.0</t>
-  </si>
-  <si>
-    <t>size_min2.0</t>
-  </si>
-  <si>
-    <t>size_min7.0</t>
-  </si>
-  <si>
-    <t>size_min12.0</t>
-  </si>
-  <si>
-    <t>size_min17.0</t>
-  </si>
-  <si>
-    <t>size_min22.0</t>
-  </si>
-  <si>
-    <t>size_min27.0</t>
-  </si>
-  <si>
-    <t>size_min32.0</t>
-  </si>
-  <si>
-    <t>size_min37.0</t>
-  </si>
-  <si>
-    <t>size_min42.0</t>
-  </si>
-  <si>
-    <t>size_min47.0</t>
+    <t>coef1213.0</t>
   </si>
 </sst>
 </file>
@@ -811,36 +781,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -857,36 +797,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -903,36 +813,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.0509259259259259</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -949,36 +829,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>9</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -995,36 +845,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>43.2</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1041,36 +861,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>509</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1087,36 +877,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2709,13 +2469,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AS11"/>
+  <dimension ref="A2:AI11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:45">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2821,175 +2581,115 @@
       <c r="AI2" t="s">
         <v>34</v>
       </c>
-      <c r="AJ2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="4" spans="1:45">
+    <row r="4" spans="1:35">
       <c r="A4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>9</v>
       </c>
       <c r="D4">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="E4">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="F4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H4">
         <v>9</v>
       </c>
       <c r="I4">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="K4">
         <v>5</v>
       </c>
       <c r="L4">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="M4">
-        <v>25</v>
+        <v>9</v>
       </c>
       <c r="N4">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="O4">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="P4">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="Q4">
-        <v>1100</v>
+        <v>7</v>
       </c>
       <c r="R4">
-        <v>2100</v>
+        <v>9</v>
       </c>
       <c r="S4">
-        <v>3100</v>
+        <v>11</v>
       </c>
       <c r="T4">
-        <v>4100</v>
+        <v>13</v>
       </c>
       <c r="U4">
-        <v>5100</v>
+        <v>5</v>
       </c>
       <c r="V4">
-        <v>6100</v>
+        <v>7</v>
       </c>
       <c r="W4">
-        <v>7100</v>
+        <v>9</v>
       </c>
       <c r="X4">
-        <v>8100</v>
+        <v>11</v>
       </c>
       <c r="Y4">
-        <v>9100</v>
+        <v>13</v>
       </c>
       <c r="Z4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <v>1</v>
       </c>
       <c r="AB4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AC4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD4">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="AE4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AF4">
-        <v>3.5</v>
+        <v>7</v>
       </c>
       <c r="AG4">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AH4">
-        <v>4.5</v>
+        <v>11</v>
       </c>
       <c r="AI4">
-        <v>5</v>
-      </c>
-      <c r="AJ4">
-        <v>2</v>
-      </c>
-      <c r="AK4">
-        <v>7</v>
-      </c>
-      <c r="AL4">
-        <v>12</v>
-      </c>
-      <c r="AM4">
-        <v>17</v>
-      </c>
-      <c r="AN4">
-        <v>22</v>
-      </c>
-      <c r="AO4">
-        <v>27</v>
-      </c>
-      <c r="AP4">
-        <v>32</v>
-      </c>
-      <c r="AQ4">
-        <v>37</v>
-      </c>
-      <c r="AR4">
-        <v>42</v>
-      </c>
-      <c r="AS4">
-        <v>47</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:45">
+    <row r="5" spans="1:35">
       <c r="A5">
         <v>9</v>
       </c>
@@ -3095,38 +2795,8 @@
       <c r="AI5">
         <v>9</v>
       </c>
-      <c r="AJ5">
-        <v>9</v>
-      </c>
-      <c r="AK5">
-        <v>9</v>
-      </c>
-      <c r="AL5">
-        <v>9</v>
-      </c>
-      <c r="AM5">
-        <v>9</v>
-      </c>
-      <c r="AN5">
-        <v>9</v>
-      </c>
-      <c r="AO5">
-        <v>9</v>
-      </c>
-      <c r="AP5">
-        <v>9</v>
-      </c>
-      <c r="AQ5">
-        <v>9</v>
-      </c>
-      <c r="AR5">
-        <v>9</v>
-      </c>
-      <c r="AS5">
-        <v>9</v>
-      </c>
     </row>
-    <row r="6" spans="1:45">
+    <row r="6" spans="1:35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3232,38 +2902,8 @@
       <c r="AI6">
         <v>0</v>
       </c>
-      <c r="AJ6">
-        <v>0</v>
-      </c>
-      <c r="AK6">
-        <v>0</v>
-      </c>
-      <c r="AL6">
-        <v>0</v>
-      </c>
-      <c r="AM6">
-        <v>0</v>
-      </c>
-      <c r="AN6">
-        <v>0</v>
-      </c>
-      <c r="AO6">
-        <v>0</v>
-      </c>
-      <c r="AP6">
-        <v>0</v>
-      </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:35">
       <c r="A7">
         <v>0.0509259259259259</v>
       </c>
@@ -3369,38 +3009,8 @@
       <c r="AI7">
         <v>0.0509259259259259</v>
       </c>
-      <c r="AJ7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AK7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AL7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AM7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AN7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AO7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AP7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AQ7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AR7">
-        <v>0.0509259259259259</v>
-      </c>
-      <c r="AS7">
-        <v>0.0509259259259259</v>
-      </c>
     </row>
-    <row r="8" spans="1:45">
+    <row r="8" spans="1:35">
       <c r="A8">
         <v>9</v>
       </c>
@@ -3506,38 +3116,8 @@
       <c r="AI8">
         <v>9</v>
       </c>
-      <c r="AJ8">
-        <v>9</v>
-      </c>
-      <c r="AK8">
-        <v>9</v>
-      </c>
-      <c r="AL8">
-        <v>9</v>
-      </c>
-      <c r="AM8">
-        <v>9</v>
-      </c>
-      <c r="AN8">
-        <v>9</v>
-      </c>
-      <c r="AO8">
-        <v>9</v>
-      </c>
-      <c r="AP8">
-        <v>9</v>
-      </c>
-      <c r="AQ8">
-        <v>9</v>
-      </c>
-      <c r="AR8">
-        <v>9</v>
-      </c>
-      <c r="AS8">
-        <v>9</v>
-      </c>
     </row>
-    <row r="9" spans="1:45">
+    <row r="9" spans="1:35">
       <c r="A9">
         <v>43.2</v>
       </c>
@@ -3643,38 +3223,8 @@
       <c r="AI9">
         <v>43.2</v>
       </c>
-      <c r="AJ9">
-        <v>43.2</v>
-      </c>
-      <c r="AK9">
-        <v>43.2</v>
-      </c>
-      <c r="AL9">
-        <v>43.2</v>
-      </c>
-      <c r="AM9">
-        <v>43.2</v>
-      </c>
-      <c r="AN9">
-        <v>43.2</v>
-      </c>
-      <c r="AO9">
-        <v>43.2</v>
-      </c>
-      <c r="AP9">
-        <v>43.2</v>
-      </c>
-      <c r="AQ9">
-        <v>43.2</v>
-      </c>
-      <c r="AR9">
-        <v>43.2</v>
-      </c>
-      <c r="AS9">
-        <v>43.2</v>
-      </c>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:35">
       <c r="A10">
         <v>509</v>
       </c>
@@ -3780,38 +3330,8 @@
       <c r="AI10">
         <v>509</v>
       </c>
-      <c r="AJ10">
-        <v>509</v>
-      </c>
-      <c r="AK10">
-        <v>509</v>
-      </c>
-      <c r="AL10">
-        <v>509</v>
-      </c>
-      <c r="AM10">
-        <v>509</v>
-      </c>
-      <c r="AN10">
-        <v>509</v>
-      </c>
-      <c r="AO10">
-        <v>509</v>
-      </c>
-      <c r="AP10">
-        <v>509</v>
-      </c>
-      <c r="AQ10">
-        <v>509</v>
-      </c>
-      <c r="AR10">
-        <v>509</v>
-      </c>
-      <c r="AS10">
-        <v>509</v>
-      </c>
     </row>
-    <row r="11" spans="1:45">
+    <row r="11" spans="1:35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3915,36 +3435,6 @@
         <v>0</v>
       </c>
       <c r="AI11">
-        <v>0</v>
-      </c>
-      <c r="AJ11">
-        <v>0</v>
-      </c>
-      <c r="AK11">
-        <v>0</v>
-      </c>
-      <c r="AL11">
-        <v>0</v>
-      </c>
-      <c r="AM11">
-        <v>0</v>
-      </c>
-      <c r="AN11">
-        <v>0</v>
-      </c>
-      <c r="AO11">
-        <v>0</v>
-      </c>
-      <c r="AP11">
-        <v>0</v>
-      </c>
-      <c r="AQ11">
-        <v>0</v>
-      </c>
-      <c r="AR11">
-        <v>0</v>
-      </c>
-      <c r="AS11">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
nouveau système d'écriture des charts dans le fichier Excel
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TF4\Documents\Baulieu\python\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -40,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,7 +84,2414 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1421124048"/>
+        <c:axId val="-1421124592"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1421124048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1421124592"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1421124592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1421124048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$6:$J$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$7:$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$8:$J$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$9:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$10:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$11:$J$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$12:$J$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1421136016"/>
+        <c:axId val="-1421138192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1421136016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1421138192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1421138192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1421136016"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$6:$O$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$7:$O$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$8:$O$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$9:$O$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$10:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$11:$O$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$12:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1421223264"/>
+        <c:axId val="-1264045200"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1421223264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264045200"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1264045200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1421223264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$6:$T$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$7:$T$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$8:$T$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$9:$T$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$10:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$11:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$12:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1264043568"/>
+        <c:axId val="-1264049008"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1264043568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264049008"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1264049008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264043568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef5</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$6:$Y$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$7:$Y$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$8:$Y$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$9:$Y$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$10:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$11:$Y$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$12:$Y$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1264051184"/>
+        <c:axId val="-1264043024"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1264051184"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264043024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1264043024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264051184"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef8</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$6:$AD$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$7:$AD$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$8:$AD$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$9:$AD$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$10:$AD$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$11:$AD$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$12:$AD$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1264046288"/>
+        <c:axId val="-1264044656"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1264046288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264044656"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1264044656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264046288"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>coef12</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>images/s</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$6:$AI$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>récupération profondeur</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$7:$AI$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.0925925925925902E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>fiabilité height</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$8:$AI$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>proportion de cibles</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$9:$AI$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>nombre de points</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$10:$AI$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>509</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>509</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>nombre de pertes</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$11:$AI$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:v>indice de performance</c:v>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$12:$AI$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-1264039760"/>
+        <c:axId val="-1264041392"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1264039760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264041392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1264041392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-1264039760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -124,7 +2537,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -156,9 +2569,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -190,6 +2604,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -365,14 +2780,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AI11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -479,7 +2894,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -586,7 +3001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9</v>
       </c>
@@ -693,7 +3108,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -800,114 +3215,114 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="B7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="C7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="D7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="E7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="F7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="G7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="H7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="I7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="J7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="K7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="L7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="M7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="N7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="O7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="P7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="Q7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="R7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="S7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="T7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="U7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="V7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="W7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="X7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="Y7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="Z7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AA7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AB7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AC7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AD7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AE7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AF7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AG7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AH7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
       <c r="AI7">
-        <v>0.0509259259259259</v>
+        <v>5.0925925925925902E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1014,7 +3429,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>43.2</v>
       </c>
@@ -1121,7 +3536,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>509</v>
       </c>
@@ -1228,7 +3643,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="11" spans="1:35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1338,4 +3753,19 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adaptation au dossier v2 sur ubuntu
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -1,21 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TF4\Documents\Baulieu\python\tests\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -46,8 +41,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,30 +79,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -126,22 +103,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$6:$E$6</c:f>
@@ -173,7 +146,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$7:$E$7</c:f>
@@ -181,19 +153,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -205,7 +177,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$8:$E$8</c:f>
@@ -213,19 +184,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -237,7 +208,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$9:$E$9</c:f>
@@ -245,19 +215,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -269,7 +239,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$10:$E$10</c:f>
@@ -277,19 +246,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -301,7 +270,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$11:$E$11</c:f>
@@ -333,59 +301,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$12:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1421124048"/>
-        <c:axId val="-1421124592"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1421124048"/>
+        <c:axId val="50010001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1421124592"/>
+        <c:crossAx val="50010002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1421124592"/>
+        <c:axId val="50010002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1421124048"/>
+        <c:crossAx val="50010001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -393,11 +344,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -409,17 +357,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -438,22 +376,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$6:$J$6</c:f>
@@ -485,7 +419,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$7:$J$7</c:f>
@@ -493,19 +426,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -517,7 +450,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$8:$J$8</c:f>
@@ -525,19 +457,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -549,7 +481,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$9:$J$9</c:f>
@@ -557,19 +488,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -581,7 +512,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$10:$J$10</c:f>
@@ -589,19 +519,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -613,7 +543,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$11:$J$11</c:f>
@@ -645,59 +574,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1421136016"/>
-        <c:axId val="-1421138192"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1421136016"/>
+        <c:axId val="50020001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1421138192"/>
+        <c:crossAx val="50020002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1421138192"/>
+        <c:axId val="50020002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1421136016"/>
+        <c:crossAx val="50020001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -705,11 +617,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -721,17 +630,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -750,22 +649,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$6:$O$6</c:f>
@@ -797,7 +692,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$7:$O$7</c:f>
@@ -805,19 +699,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -829,7 +723,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$8:$O$8</c:f>
@@ -837,19 +730,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,7 +754,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$9:$O$9</c:f>
@@ -869,19 +761,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -893,7 +785,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$10:$O$10</c:f>
@@ -901,19 +792,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -925,7 +816,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$11:$O$11</c:f>
@@ -957,59 +847,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1421223264"/>
-        <c:axId val="-1264045200"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50030001"/>
+        <c:axId val="50030002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1421223264"/>
+        <c:axId val="50030001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264045200"/>
+        <c:crossAx val="50030002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1264045200"/>
+        <c:axId val="50030002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1421223264"/>
+        <c:crossAx val="50030001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1017,11 +890,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1033,17 +903,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1062,22 +922,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$6:$T$6</c:f>
@@ -1109,7 +965,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$7:$T$7</c:f>
@@ -1117,19 +972,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1141,7 +996,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$8:$T$8</c:f>
@@ -1149,19 +1003,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1173,7 +1027,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$9:$T$9</c:f>
@@ -1181,19 +1034,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1205,7 +1058,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$10:$T$10</c:f>
@@ -1213,19 +1065,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1237,7 +1089,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$11:$T$11</c:f>
@@ -1269,59 +1120,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$12:$T$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1264043568"/>
-        <c:axId val="-1264049008"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50040001"/>
+        <c:axId val="50040002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1264043568"/>
+        <c:axId val="50040001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264049008"/>
+        <c:crossAx val="50040002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1264049008"/>
+        <c:axId val="50040002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264043568"/>
+        <c:crossAx val="50040001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1329,11 +1163,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1345,17 +1176,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1374,22 +1195,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$6:$Y$6</c:f>
@@ -1421,7 +1238,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$7:$Y$7</c:f>
@@ -1429,19 +1245,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1453,7 +1269,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$8:$Y$8</c:f>
@@ -1461,19 +1276,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1485,7 +1300,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$9:$Y$9</c:f>
@@ -1493,19 +1307,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1517,7 +1331,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$10:$Y$10</c:f>
@@ -1525,19 +1338,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1549,7 +1362,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$11:$Y$11</c:f>
@@ -1581,59 +1393,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$12:$Y$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1264051184"/>
-        <c:axId val="-1264043024"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50050001"/>
+        <c:axId val="50050002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1264051184"/>
+        <c:axId val="50050001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264043024"/>
+        <c:crossAx val="50050002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1264043024"/>
+        <c:axId val="50050002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264051184"/>
+        <c:crossAx val="50050001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1641,11 +1436,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1657,17 +1449,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1686,22 +1468,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$6:$AD$6</c:f>
@@ -1733,7 +1511,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$7:$AD$7</c:f>
@@ -1741,19 +1518,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1765,7 +1542,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$8:$AD$8</c:f>
@@ -1773,19 +1549,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1797,7 +1573,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$9:$AD$9</c:f>
@@ -1805,19 +1580,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1829,7 +1604,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$10:$AD$10</c:f>
@@ -1837,19 +1611,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1861,7 +1635,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$11:$AD$11</c:f>
@@ -1893,59 +1666,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$12:$AD$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1264046288"/>
-        <c:axId val="-1264044656"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50060001"/>
+        <c:axId val="50060002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1264046288"/>
+        <c:axId val="50060001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264044656"/>
+        <c:crossAx val="50060002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1264044656"/>
+        <c:axId val="50060002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264046288"/>
+        <c:crossAx val="50060001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1953,11 +1709,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1969,17 +1722,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1998,22 +1741,18 @@
         </c:rich>
       </c:tx>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:title>
-    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$6:$AI$6</c:f>
@@ -2045,7 +1784,6 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$7:$AI$7</c:f>
@@ -2053,19 +1791,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0925925925925902E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0925925925925902E-2</c:v>
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2077,7 +1815,6 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$8:$AI$8</c:f>
@@ -2085,19 +1822,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2109,7 +1846,6 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$9:$AI$9</c:f>
@@ -2117,19 +1853,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>43.2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>43.2</c:v>
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,7 +1877,6 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$10:$AI$10</c:f>
@@ -2149,19 +1884,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>509</c:v>
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2173,7 +1908,6 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$11:$AI$11</c:f>
@@ -2205,59 +1939,42 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
-          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$12:$AI$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-1264039760"/>
-        <c:axId val="-1264041392"/>
+                <c:ptCount val="1"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="50070001"/>
+        <c:axId val="50070002"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1264039760"/>
+        <c:axId val="50070001"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264041392"/>
+        <c:crossAx val="50070002"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1264041392"/>
+        <c:axId val="50070002"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1264039760"/>
+        <c:crossAx val="50070001"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2265,11 +1982,8 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
-      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2284,15 +1998,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2313,16 +2027,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2343,16 +2057,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2373,16 +2087,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2403,16 +2117,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2433,16 +2147,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2463,16 +2177,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2537,7 +2251,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2569,10 +2283,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2604,7 +2317,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2780,14 +2492,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AI11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2894,7 +2606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -3001,114 +2713,114 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35">
       <c r="A5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Q5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="R5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="S5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="T5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="U5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="V5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="W5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="X5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Y5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Z5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AA5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AB5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AC5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AD5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AE5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AF5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AG5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AH5">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AI5">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35">
       <c r="A6">
         <v>0</v>
       </c>
@@ -3215,435 +2927,435 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35">
       <c r="A7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="B7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="J7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="K7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="L7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="M7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="O7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="P7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="Q7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="R7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="S7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="T7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="U7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="V7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="W7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="X7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="Y7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="Z7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AA7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AB7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AC7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AD7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AF7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AG7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AH7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
       <c r="AI7">
-        <v>5.0925925925925902E-2</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35">
       <c r="A8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="I8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="J8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="M8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="N8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="O8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="P8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Q8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="R8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="S8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="T8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="U8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="V8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="W8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="X8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Y8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="Z8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AA8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AB8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AC8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AD8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AE8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AF8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AG8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AH8">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AI8">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35">
       <c r="A9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="B9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="C9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="D9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="E9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="F9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="G9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="H9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="I9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="J9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="K9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="L9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="M9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="N9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="O9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="P9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="Q9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="R9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="S9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="T9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="U9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="V9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="W9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="X9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="Y9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="Z9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AA9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AB9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AC9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AD9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AE9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AF9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AG9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AH9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
       <c r="AI9">
-        <v>43.2</v>
+        <v>0.4</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35">
       <c r="A10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="B10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="D10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="E10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="F10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="G10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="H10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="I10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="J10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="K10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="L10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="M10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="N10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="O10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="P10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="Q10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="R10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="S10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="T10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="U10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="V10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="W10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="X10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="Y10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="Z10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AA10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AB10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AC10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AD10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AE10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AF10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AG10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AH10">
-        <v>509</v>
+        <v>16</v>
       </c>
       <c r="AI10">
-        <v>509</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35">
       <c r="A11">
         <v>0</v>
       </c>
@@ -3756,14 +3468,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
mise à niveau du calcul des KPIs
</commit_message>
<xml_diff>
--- a/analyse.xlsx
+++ b/analyse.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TF4\Documents\Baulieu\python\tests\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
@@ -10,7 +15,7 @@
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="charts" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -41,8 +46,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,12 +84,30 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -103,18 +126,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$6:$E$6</c:f>
@@ -146,6 +173,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$7:$E$7</c:f>
@@ -156,16 +184,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.258620689655172</c:v>
+                  <c:v>0.25862068965517199</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0178571428571429</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0217391304347826</c:v>
+                  <c:v>1.7857142857142901E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1739130434782601E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -177,6 +205,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$8:$E$8</c:f>
@@ -208,6 +237,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$9:$E$9</c:f>
@@ -227,7 +257,7 @@
                   <c:v>11.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -239,9 +269,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$A$10:$E$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$A$15:$E$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -270,6 +301,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$11:$E$11</c:f>
@@ -301,42 +333,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$A$12:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50010001"/>
-        <c:axId val="50010002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712612000"/>
+        <c:axId val="1712622336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50010001"/>
+        <c:axId val="1712612000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010002"/>
+        <c:crossAx val="1712622336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50010002"/>
+        <c:axId val="1712622336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50010001"/>
+        <c:crossAx val="1712612000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -344,8 +393,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -357,7 +409,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -376,18 +438,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$6:$J$6</c:f>
@@ -419,6 +485,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$7:$J$7</c:f>
@@ -429,10 +496,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.562874251497006</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.562841530054645</c:v>
+                  <c:v>0.56287425149700598</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.56284153005464499</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -450,6 +517,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$8:$J$8</c:f>
@@ -481,6 +549,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$9:$J$9</c:f>
@@ -512,9 +581,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$F$10:$J$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$15:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -543,6 +613,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$11:$J$11</c:f>
@@ -574,42 +645,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$F$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50020001"/>
-        <c:axId val="50020002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712609824"/>
+        <c:axId val="1712611456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50020001"/>
+        <c:axId val="1712609824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020002"/>
+        <c:crossAx val="1712611456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50020002"/>
+        <c:axId val="1712611456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50020001"/>
+        <c:crossAx val="1712609824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -617,8 +705,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -630,7 +721,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -649,18 +750,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$6:$O$6</c:f>
@@ -692,6 +797,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$7:$O$7</c:f>
@@ -702,16 +808,16 @@
                   <c:v>0.547619047619048</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0338983050847458</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0169491525423729</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0185185185185185</c:v>
+                  <c:v>3.3898305084745797E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6949152542372899E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.85185185185185E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,6 +829,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$8:$O$8</c:f>
@@ -754,6 +861,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$9:$O$9</c:f>
@@ -785,9 +893,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$K$10:$O$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$15:$O$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -816,6 +925,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$11:$O$11</c:f>
@@ -847,42 +957,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$K$12:$O$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50030001"/>
-        <c:axId val="50030002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712610368"/>
+        <c:axId val="1712614720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50030001"/>
+        <c:axId val="1712610368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030002"/>
+        <c:crossAx val="1712614720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50030002"/>
+        <c:axId val="1712614720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50030001"/>
+        <c:crossAx val="1712610368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -890,8 +1017,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -903,7 +1033,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -922,18 +1062,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$6:$T$6</c:f>
@@ -965,6 +1109,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$7:$T$7</c:f>
@@ -972,13 +1117,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.0181818181818182</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0208333333333333</c:v>
+                  <c:v>1.8181818181818198E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0833333333333301E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.02</c:v>
@@ -996,6 +1141,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$8:$T$8</c:f>
@@ -1027,6 +1173,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$9:$T$9</c:f>
@@ -1058,9 +1205,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$P$10:$T$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$P$15:$T$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1089,6 +1237,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$11:$T$11</c:f>
@@ -1120,42 +1269,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$P$12:$T$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50040001"/>
-        <c:axId val="50040002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712612544"/>
+        <c:axId val="1712613088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50040001"/>
+        <c:axId val="1712612544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040002"/>
+        <c:crossAx val="1712613088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50040002"/>
+        <c:axId val="1712613088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50040001"/>
+        <c:crossAx val="1712612544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1163,8 +1329,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1176,7 +1345,17 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1195,18 +1374,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$6:$Y$6</c:f>
@@ -1238,6 +1421,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$7:$Y$7</c:f>
@@ -1248,13 +1432,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0192307692307692</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0227272727272727</c:v>
+                  <c:v>1.9230769230769201E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.27272727272727E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1269,6 +1453,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$8:$Y$8</c:f>
@@ -1300,6 +1485,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$9:$Y$9</c:f>
@@ -1316,7 +1502,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.8</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>11</c:v>
@@ -1331,9 +1517,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$U$10:$Y$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$U$15:$Y$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1362,6 +1549,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$11:$Y$11</c:f>
@@ -1393,42 +1581,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$U$12:$Y$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50050001"/>
-        <c:axId val="50050002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712619616"/>
+        <c:axId val="1712620704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50050001"/>
+        <c:axId val="1712619616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050002"/>
+        <c:crossAx val="1712620704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50050002"/>
+        <c:axId val="1712620704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50050001"/>
+        <c:crossAx val="1712619616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1436,8 +1641,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1449,7 +1657,17 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1468,18 +1686,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$6:$AD$6</c:f>
@@ -1511,6 +1733,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$7:$AD$7</c:f>
@@ -1524,7 +1747,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0208333333333333</c:v>
+                  <c:v>2.0833333333333301E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -1542,6 +1765,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$8:$AD$8</c:f>
@@ -1573,6 +1797,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$9:$AD$9</c:f>
@@ -1592,7 +1817,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.2</c:v>
+                  <c:v>9.1999999999999993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,9 +1829,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$Z$10:$AD$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$Z$15:$AD$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1635,6 +1861,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$11:$AD$11</c:f>
@@ -1666,42 +1893,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$Z$12:$AD$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50060001"/>
-        <c:axId val="50060002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712616896"/>
+        <c:axId val="1712623424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50060001"/>
+        <c:axId val="1712616896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50060002"/>
+        <c:crossAx val="1712623424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50060002"/>
+        <c:axId val="1712623424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50060001"/>
+        <c:crossAx val="1712616896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1709,8 +1953,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1722,7 +1969,17 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1741,18 +1998,22 @@
         </c:rich>
       </c:tx>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:v>images/s</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$6:$AI$6</c:f>
@@ -1784,6 +2045,7 @@
           <c:tx>
             <c:v>récupération profondeur</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$7:$AI$7</c:f>
@@ -1794,7 +2056,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0178571428571429</c:v>
+                  <c:v>1.7857142857142901E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1815,6 +2077,7 @@
           <c:tx>
             <c:v>fiabilité height</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$8:$AI$8</c:f>
@@ -1846,6 +2109,7 @@
           <c:tx>
             <c:v>proportion de cibles</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$9:$AI$9</c:f>
@@ -1877,9 +2141,10 @@
           <c:tx>
             <c:v>nombre de points</c:v>
           </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>data!$AE$10:$AI$10</c:f>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$AE$15:$AI$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1908,6 +2173,7 @@
           <c:tx>
             <c:v>nombre de pertes</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$11:$AI$11</c:f>
@@ -1939,42 +2205,59 @@
           <c:tx>
             <c:v>indice de performance</c:v>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>data!$AE$12:$AI$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="50070001"/>
-        <c:axId val="50070002"/>
+                <c:ptCount val="5"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1712619072"/>
+        <c:axId val="1552886144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="50070001"/>
+        <c:axId val="1712619072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50070002"/>
+        <c:crossAx val="1552886144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="50070002"/>
+        <c:axId val="1552886144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50070001"/>
+        <c:crossAx val="1712619072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1982,8 +2265,11 @@
     <c:legend>
       <c:legendPos val="r"/>
       <c:layout/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1997,16 +2283,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2027,16 +2313,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2057,16 +2343,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2089,14 +2375,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2117,16 +2403,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2147,16 +2433,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2177,16 +2463,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2251,7 +2537,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2283,9 +2569,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2317,6 +2604,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2492,14 +2780,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:AI11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2606,7 +2896,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2713,7 +3003,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>13</v>
       </c>
@@ -2820,7 +3110,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -2927,30 +3217,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>0</v>
       </c>
       <c r="B7">
-        <v>0.258620689655172</v>
+        <v>0.25862068965517199</v>
       </c>
       <c r="C7">
         <v>0.02</v>
       </c>
       <c r="D7">
-        <v>0.0178571428571429</v>
+        <v>1.7857142857142901E-2</v>
       </c>
       <c r="E7">
-        <v>0.0217391304347826</v>
+        <v>2.1739130434782601E-2</v>
       </c>
       <c r="F7">
         <v>0</v>
       </c>
       <c r="G7">
-        <v>0.562874251497006</v>
+        <v>0.56287425149700598</v>
       </c>
       <c r="H7">
-        <v>0.562841530054645</v>
+        <v>0.56284153005464499</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -2962,25 +3252,25 @@
         <v>0.547619047619048</v>
       </c>
       <c r="L7">
-        <v>0.0338983050847458</v>
+        <v>3.3898305084745797E-2</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
-        <v>0.0169491525423729</v>
+        <v>1.6949152542372899E-2</v>
       </c>
       <c r="O7">
-        <v>0.0185185185185185</v>
+        <v>1.85185185185185E-2</v>
       </c>
       <c r="P7">
-        <v>0.0181818181818182</v>
+        <v>1.8181818181818198E-2</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0.0208333333333333</v>
+        <v>2.0833333333333301E-2</v>
       </c>
       <c r="S7">
         <v>0.02</v>
@@ -2992,13 +3282,13 @@
         <v>0</v>
       </c>
       <c r="V7">
-        <v>0.0192307692307692</v>
+        <v>1.9230769230769201E-2</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7">
-        <v>0.0227272727272727</v>
+        <v>2.27272727272727E-2</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -3010,7 +3300,7 @@
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>0.0208333333333333</v>
+        <v>2.0833333333333301E-2</v>
       </c>
       <c r="AC7">
         <v>0</v>
@@ -3022,7 +3312,7 @@
         <v>0</v>
       </c>
       <c r="AF7">
-        <v>0.0178571428571429</v>
+        <v>1.7857142857142901E-2</v>
       </c>
       <c r="AG7">
         <v>0</v>
@@ -3034,7 +3324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>13</v>
       </c>
@@ -3141,7 +3431,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>10.8</v>
       </c>
@@ -3155,7 +3445,7 @@
         <v>11.2</v>
       </c>
       <c r="E9">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F9">
         <v>11.4</v>
@@ -3212,7 +3502,7 @@
         <v>12</v>
       </c>
       <c r="X9">
-        <v>8.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="Y9">
         <v>11</v>
@@ -3230,7 +3520,7 @@
         <v>11</v>
       </c>
       <c r="AD9">
-        <v>9.2</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="AE9">
         <v>9.6</v>
@@ -3248,218 +3538,360 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f>A15/100</f>
+        <v>2.33</v>
+      </c>
+      <c r="B10">
+        <f t="shared" ref="B10:AI10" si="0">B15/100</f>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>2.27</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>1.72</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>2.17</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>2.29</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1.58</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>2.27</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>2.35</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>2.33</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="0"/>
+        <v>2.36</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="0"/>
+        <v>2.33</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="0"/>
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="0"/>
+        <v>2.33</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="0"/>
+        <v>2.36</v>
+      </c>
+      <c r="AB10">
+        <f t="shared" si="0"/>
+        <v>2.34</v>
+      </c>
+      <c r="AC10">
+        <f t="shared" si="0"/>
+        <v>2.33</v>
+      </c>
+      <c r="AD10">
+        <f t="shared" si="0"/>
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="AE10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AF10">
+        <f t="shared" si="0"/>
+        <v>2.35</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="0"/>
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="0"/>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="0"/>
+        <v>2.27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11">
+        <v>0</v>
+      </c>
+      <c r="AD11">
+        <v>0</v>
+      </c>
+      <c r="AE11">
+        <v>0</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0</v>
+      </c>
+      <c r="AH11">
+        <v>0</v>
+      </c>
+      <c r="AI11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A15">
         <v>233</v>
       </c>
-      <c r="B10">
+      <c r="B15">
         <v>228</v>
       </c>
-      <c r="C10">
+      <c r="C15">
         <v>232</v>
       </c>
-      <c r="D10">
+      <c r="D15">
         <v>234</v>
       </c>
-      <c r="E10">
+      <c r="E15">
         <v>232</v>
       </c>
-      <c r="F10">
+      <c r="F15">
         <v>227</v>
       </c>
-      <c r="G10">
+      <c r="G15">
         <v>172</v>
       </c>
-      <c r="H10">
+      <c r="H15">
         <v>217</v>
       </c>
-      <c r="I10">
+      <c r="I15">
         <v>225</v>
       </c>
-      <c r="J10">
+      <c r="J15">
         <v>229</v>
       </c>
-      <c r="K10">
+      <c r="K15">
         <v>158</v>
       </c>
-      <c r="L10">
+      <c r="L15">
         <v>224</v>
       </c>
-      <c r="M10">
+      <c r="M15">
         <v>227</v>
       </c>
-      <c r="N10">
+      <c r="N15">
         <v>232</v>
       </c>
-      <c r="O10">
+      <c r="O15">
         <v>225</v>
       </c>
-      <c r="P10">
+      <c r="P15">
         <v>232</v>
       </c>
-      <c r="Q10">
+      <c r="Q15">
         <v>234</v>
       </c>
-      <c r="R10">
+      <c r="R15">
         <v>235</v>
       </c>
-      <c r="S10">
+      <c r="S15">
         <v>233</v>
       </c>
-      <c r="T10">
+      <c r="T15">
         <v>234</v>
       </c>
-      <c r="U10">
+      <c r="U15">
         <v>224</v>
       </c>
-      <c r="V10">
+      <c r="V15">
         <v>236</v>
       </c>
-      <c r="W10">
+      <c r="W15">
         <v>233</v>
       </c>
-      <c r="X10">
+      <c r="X15">
         <v>228</v>
       </c>
-      <c r="Y10">
+      <c r="Y15">
         <v>224</v>
       </c>
-      <c r="Z10">
+      <c r="Z15">
         <v>233</v>
       </c>
-      <c r="AA10">
+      <c r="AA15">
         <v>236</v>
       </c>
-      <c r="AB10">
+      <c r="AB15">
         <v>234</v>
       </c>
-      <c r="AC10">
+      <c r="AC15">
         <v>233</v>
       </c>
-      <c r="AD10">
+      <c r="AD15">
         <v>224</v>
       </c>
-      <c r="AE10">
+      <c r="AE15">
         <v>232</v>
       </c>
-      <c r="AF10">
+      <c r="AF15">
         <v>235</v>
       </c>
-      <c r="AG10">
+      <c r="AG15">
         <v>232</v>
       </c>
-      <c r="AH10">
+      <c r="AH15">
         <v>230</v>
       </c>
-      <c r="AI10">
+      <c r="AI15">
         <v>227</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11">
-        <v>0</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11">
-        <v>0</v>
-      </c>
-      <c r="V11">
-        <v>0</v>
-      </c>
-      <c r="W11">
-        <v>0</v>
-      </c>
-      <c r="X11">
-        <v>0</v>
-      </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11">
-        <v>0</v>
-      </c>
-      <c r="AB11">
-        <v>0</v>
-      </c>
-      <c r="AC11">
-        <v>0</v>
-      </c>
-      <c r="AD11">
-        <v>0</v>
-      </c>
-      <c r="AE11">
-        <v>0</v>
-      </c>
-      <c r="AF11">
-        <v>0</v>
-      </c>
-      <c r="AG11">
-        <v>0</v>
-      </c>
-      <c r="AH11">
-        <v>0</v>
-      </c>
-      <c r="AI11">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3468,12 +3900,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>